<commit_message>
Time to Update.  Board layout started.
</commit_message>
<xml_diff>
--- a/Parts_List.xlsx
+++ b/Parts_List.xlsx
@@ -16,6 +16,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Parts_List!$A$1:$J$53</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">Parts_List!$1:$1</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
@@ -276,27 +277,12 @@
     <t>Sullins</t>
   </si>
   <si>
-    <t>PPTC081LFBN-RC</t>
-  </si>
-  <si>
-    <t>CONN HEADER FEMALE 8POS .1" TIN</t>
-  </si>
-  <si>
-    <t>SULLINS_PPTC081LFBN-RC</t>
-  </si>
-  <si>
     <t>part number for stepstick interface</t>
   </si>
   <si>
-    <t>PPTC202LFBN-RC</t>
-  </si>
-  <si>
     <t>CONN HEADER FEM 40POS .1" DL TIN</t>
   </si>
   <si>
-    <t>SULLINS_PPTC202LFBN-RC</t>
-  </si>
-  <si>
     <t>L</t>
   </si>
   <si>
@@ -541,6 +527,21 @@
   </si>
   <si>
     <t>SOT95P280X145-5N</t>
+  </si>
+  <si>
+    <t>PPPC081LFBN-RC</t>
+  </si>
+  <si>
+    <t>PPPC202LFBN-RC</t>
+  </si>
+  <si>
+    <t>CONN HEADER FEMALE 8POS .1" G</t>
+  </si>
+  <si>
+    <t>SULLINS_PPxC202LFBN-RC</t>
+  </si>
+  <si>
+    <t>SULLINS_PPxC081LFBN-RC</t>
   </si>
 </sst>
 </file>
@@ -1408,8 +1409,8 @@
   <dimension ref="A1:K53"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C26" sqref="C26"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1954,7 +1955,7 @@
         <v>3</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>16</v>
@@ -2090,7 +2091,7 @@
         <v>3</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="G20" s="2" t="s">
         <v>16</v>
@@ -2158,7 +2159,7 @@
         <v>1</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="G22" s="2" t="s">
         <v>16</v>
@@ -2183,16 +2184,16 @@
         <v>83</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="E23" s="2">
         <v>4</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="G23" s="2" t="s">
         <v>16</v>
@@ -2217,16 +2218,16 @@
         <v>83</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="E24" s="2">
         <v>4</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="G24" s="2" t="s">
         <v>16</v>
@@ -2249,16 +2250,16 @@
         <v>83</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="E25" s="2">
         <v>4</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="G25" s="2" t="s">
         <v>16</v>
@@ -2360,7 +2361,7 @@
         <v>1</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="G28" s="2" t="s">
         <v>16</v>
@@ -2419,16 +2420,16 @@
         <v>83</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>84</v>
+        <v>168</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>85</v>
+        <v>170</v>
       </c>
       <c r="E30" s="2">
         <v>8</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>86</v>
+        <v>172</v>
       </c>
       <c r="G30" s="2" t="s">
         <v>16</v>
@@ -2441,10 +2442,10 @@
       </c>
       <c r="J30" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>SULLINS_PPTC081LFBN-RC.kicad_mod</v>
+        <v>SULLINS_PPxC081LFBN-RC.kicad_mod</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
@@ -2455,16 +2456,16 @@
         <v>83</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>88</v>
+        <v>169</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="E31" s="2">
         <v>1</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>90</v>
+        <v>171</v>
       </c>
       <c r="G31" s="2" t="s">
         <v>16</v>
@@ -2477,28 +2478,28 @@
       </c>
       <c r="J31" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>SULLINS_PPTC202LFBN-RC.kicad_mod</v>
+        <v>SULLINS_PPxC202LFBN-RC.kicad_mod</v>
       </c>
       <c r="K31" s="2"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="E32" s="2">
         <v>1</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="G32" s="2" t="s">
         <v>16</v>
@@ -2507,7 +2508,7 @@
         <v>16</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="J32" s="3" t="str">
         <f t="shared" si="2"/>
@@ -2517,22 +2518,22 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B33" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C33" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C33" s="2" t="s">
-        <v>97</v>
-      </c>
       <c r="D33" s="2" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="E33" s="2">
         <v>1</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="G33" s="2" t="s">
         <v>16</v>
@@ -2541,7 +2542,7 @@
         <v>16</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="J33" s="3" t="str">
         <f t="shared" si="2"/>
@@ -2551,22 +2552,22 @@
     </row>
     <row r="34" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="E34" s="2">
         <v>7</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="G34" s="2" t="s">
         <v>16</v>
@@ -2575,7 +2576,7 @@
         <v>16</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="J34" s="3" t="str">
         <f t="shared" si="2"/>
@@ -2585,22 +2586,22 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="E35" s="2">
         <v>4</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="G35" s="2" t="s">
         <v>16</v>
@@ -2609,7 +2610,7 @@
         <v>16</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="J35" s="3" t="str">
         <f t="shared" si="2"/>
@@ -2619,22 +2620,22 @@
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="B36" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C36" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="C36" s="2" t="s">
-        <v>111</v>
-      </c>
       <c r="D36" s="2" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="E36" s="2">
         <v>4</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="G36" s="2" t="s">
         <v>16</v>
@@ -2643,7 +2644,7 @@
         <v>16</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="J36" s="3" t="str">
         <f t="shared" si="2"/>
@@ -2653,22 +2654,22 @@
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="E37" s="2">
         <v>1</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="G37" s="2" t="s">
         <v>16</v>
@@ -2677,7 +2678,7 @@
         <v>16</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="J37" s="3" t="str">
         <f t="shared" si="2"/>
@@ -2687,22 +2688,22 @@
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="E38" s="2">
         <v>1</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="G38" s="2" t="s">
         <v>16</v>
@@ -2711,7 +2712,7 @@
         <v>16</v>
       </c>
       <c r="I38" s="2" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="J38" s="3" t="str">
         <f t="shared" si="2"/>
@@ -2721,22 +2722,22 @@
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="E39" s="2">
         <v>1</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="G39" s="2" t="s">
         <v>16</v>
@@ -2745,7 +2746,7 @@
         <v>16</v>
       </c>
       <c r="I39" s="2" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="J39" s="3" t="str">
         <f t="shared" si="2"/>
@@ -2755,22 +2756,22 @@
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="E40" s="2">
         <v>1</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="G40" s="2" t="s">
         <v>16</v>
@@ -2779,7 +2780,7 @@
         <v>16</v>
       </c>
       <c r="I40" s="2" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="J40" s="3" t="str">
         <f t="shared" si="2"/>
@@ -2789,22 +2790,22 @@
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="E41" s="2">
         <v>4</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="G41" s="2" t="s">
         <v>16</v>
@@ -2813,7 +2814,7 @@
         <v>16</v>
       </c>
       <c r="I41" s="2" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="J41" s="3" t="str">
         <f t="shared" si="2"/>
@@ -2823,22 +2824,22 @@
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="E42" s="2">
         <v>1</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="G42" s="2" t="s">
         <v>16</v>
@@ -2847,7 +2848,7 @@
         <v>16</v>
       </c>
       <c r="I42" s="2" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="J42" s="3" t="str">
         <f t="shared" si="2"/>
@@ -2857,22 +2858,22 @@
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="E43" s="2">
         <v>1</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="G43" s="2" t="s">
         <v>16</v>
@@ -2881,7 +2882,7 @@
         <v>16</v>
       </c>
       <c r="I43" s="2" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="J43" s="3" t="str">
         <f t="shared" si="2"/>
@@ -2891,22 +2892,22 @@
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="E44" s="2">
         <v>10</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="G44" s="2" t="s">
         <v>16</v>
@@ -2915,7 +2916,7 @@
         <v>16</v>
       </c>
       <c r="I44" s="2" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="J44" s="3" t="str">
         <f t="shared" si="2"/>
@@ -2925,22 +2926,22 @@
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="E45" s="2">
         <v>1</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="G45" s="2" t="s">
         <v>16</v>
@@ -2949,7 +2950,7 @@
         <v>16</v>
       </c>
       <c r="I45" s="2" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="J45" s="3" t="str">
         <f t="shared" si="2"/>
@@ -2959,22 +2960,22 @@
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="E46" s="2">
         <v>1</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="G46" s="2" t="s">
         <v>16</v>
@@ -2983,7 +2984,7 @@
         <v>16</v>
       </c>
       <c r="I46" s="2" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="J46" s="3" t="str">
         <f t="shared" si="2"/>
@@ -2993,22 +2994,22 @@
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="E47" s="2">
         <v>2</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="G47" s="2" t="s">
         <v>16</v>
@@ -3017,7 +3018,7 @@
         <v>16</v>
       </c>
       <c r="I47" s="2" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="J47" s="3" t="str">
         <f t="shared" si="2"/>
@@ -3027,22 +3028,22 @@
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="E48" s="2">
         <v>2</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="G48" s="2" t="s">
         <v>16</v>
@@ -3051,7 +3052,7 @@
         <v>16</v>
       </c>
       <c r="I48" s="2" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="J48" s="3" t="str">
         <f t="shared" si="2"/>
@@ -3061,20 +3062,20 @@
     </row>
     <row r="49" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="E49" s="2"/>
       <c r="F49" s="2" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="G49" s="2" t="s">
         <v>16</v>
@@ -3083,7 +3084,7 @@
         <v>16</v>
       </c>
       <c r="I49" s="2" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="J49" s="3" t="str">
         <f t="shared" si="2"/>
@@ -3093,22 +3094,22 @@
     </row>
     <row r="50" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="E50" s="2">
         <v>1</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="G50" s="2" t="s">
         <v>16</v>
@@ -3117,7 +3118,7 @@
         <v>16</v>
       </c>
       <c r="I50" s="2" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="J50" s="3" t="str">
         <f t="shared" si="2"/>
@@ -3127,22 +3128,22 @@
     </row>
     <row r="51" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="E51" s="2">
         <v>1</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="G51" s="2" t="s">
         <v>16</v>
@@ -3151,7 +3152,7 @@
         <v>16</v>
       </c>
       <c r="I51" s="2" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="J51" s="3" t="str">
         <f t="shared" si="2"/>
@@ -3161,22 +3162,22 @@
     </row>
     <row r="52" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="E52" s="2">
         <v>1</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="G52" s="2" t="s">
         <v>16</v>
@@ -3185,7 +3186,7 @@
         <v>16</v>
       </c>
       <c r="I52" s="2" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="J52" s="3" t="str">
         <f t="shared" si="2"/>
@@ -3195,22 +3196,22 @@
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="E53" s="2">
         <v>4</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="G53" s="2" t="s">
         <v>16</v>

</xml_diff>